<commit_message>
Add Mean and Standard Deviation
</commit_message>
<xml_diff>
--- a/case_study/experiments/policy1Hz/multi/adversarial/KeepRight.xlsx
+++ b/case_study/experiments/policy1Hz/multi/adversarial/KeepRight.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nicopellegrinelli\abz2025_casestudy_autonomous_driving\enforcement\data\multi\adversarial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nico.pellegrinelli\Desktop\RepoLocaliGit\abz2025_casestudy_autonomous_driving\case_study\experiments\policy1Hz\multi\adversarial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78933D0-9A5F-4399-9DB4-DE9CB3D086B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B167B9-3010-40AC-89B6-04E63CA02CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="26">
   <si>
     <t>execution_id</t>
   </si>
@@ -89,6 +102,15 @@
   </si>
   <si>
     <t>40f66c97-5cde-4f12-bf37-10318158c0ea</t>
+  </si>
+  <si>
+    <t>N. crash:</t>
+  </si>
+  <si>
+    <t>Mean:</t>
+  </si>
+  <si>
+    <t>Standard Deviation:</t>
   </si>
 </sst>
 </file>
@@ -451,15 +473,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:P51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -559,7 +581,7 @@
         <v>17015.352708999671</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -609,7 +631,7 @@
         <v>17925.252387</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -659,7 +681,7 @@
         <v>17662.827208000181</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -709,7 +731,7 @@
         <v>17693.70813400019</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -759,7 +781,7 @@
         <v>17408.296651000001</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -809,7 +831,7 @@
         <v>17809.769266999869</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -859,7 +881,7 @@
         <v>17590.015179999678</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -909,7 +931,7 @@
         <v>17570.92976400008</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -959,7 +981,7 @@
         <v>17702.003270000201</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1009,7 +1031,7 @@
         <v>17369.966593000299</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1059,7 +1081,7 @@
         <v>17548.7193279987</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1109,7 +1131,7 @@
         <v>17874.451043999219</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1159,7 +1181,7 @@
         <v>17269.275488999479</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1209,7 +1231,7 @@
         <v>17824.060548000489</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1259,7 +1281,7 @@
         <v>17211.797639</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1309,7 +1331,7 @@
         <v>18267.535283001049</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1359,7 +1381,7 @@
         <v>17023.713864999081</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1409,7 +1431,7 @@
         <v>18061.26798600053</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1459,7 +1481,7 @@
         <v>17018.903575000881</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1509,7 +1531,7 @@
         <v>1598.837519999506</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1559,7 +1581,7 @@
         <v>17423.793916999781</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1609,7 +1631,7 @@
         <v>17783.331444999931</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1659,7 +1681,7 @@
         <v>17199.123564001638</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1709,7 +1731,7 @@
         <v>18313.423773000981</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +1781,7 @@
         <v>18586.998790000511</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1809,7 +1831,7 @@
         <v>18013.29699300004</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1859,7 +1881,7 @@
         <v>17195.212096999971</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1909,7 +1931,7 @@
         <v>17970.707466000022</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1959,7 +1981,7 @@
         <v>17114.072502999989</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2009,7 +2031,7 @@
         <v>18098.96916300022</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2059,7 +2081,7 @@
         <v>18516.107980000019</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2109,7 +2131,7 @@
         <v>17473.30939200037</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2159,7 +2181,7 @@
         <v>18022.38033300091</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2209,7 +2231,7 @@
         <v>18085.255308998971</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2259,7 +2281,7 @@
         <v>17503.33113899978</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2309,7 +2331,7 @@
         <v>17543.090957000459</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2359,7 +2381,7 @@
         <v>17701.102729999551</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2409,7 +2431,7 @@
         <v>17669.29492800045</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2459,7 +2481,7 @@
         <v>17611.151629998862</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2509,7 +2531,7 @@
         <v>17861.36527300005</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -2559,7 +2581,7 @@
         <v>17645.6813650002</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2609,7 +2631,7 @@
         <v>1301.5820559994611</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2659,7 +2681,7 @@
         <v>18611.988179998662</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2709,7 +2731,7 @@
         <v>17201.321901999108</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>22</v>
       </c>
@@ -2759,7 +2781,7 @@
         <v>17559.154497999771</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -2809,7 +2831,7 @@
         <v>17247.42271900141</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2881,7 @@
         <v>18276.143478999071</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -2909,7 +2931,7 @@
         <v>17279.103089998898</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -2959,7 +2981,7 @@
         <v>17913.180124998689</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -3007,6 +3029,97 @@
       </c>
       <c r="P51">
         <v>17390.513861999349</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53">
+        <f>COUNTIF(G2:G51,"True")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54">
+        <f t="shared" ref="H54" si="0">AVERAGE(H2:H51)</f>
+        <v>0.583788987426758</v>
+      </c>
+      <c r="I54">
+        <f t="shared" ref="I54:P54" si="1">AVERAGE(I2:I51)</f>
+        <v>1.9336125161743172</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="1"/>
+        <v>96.32</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="1"/>
+        <v>48.32</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="1"/>
+        <v>12.415287699977853</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="1"/>
+        <v>3.5412556000301265</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="1"/>
+        <v>2127.8618473002007</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="1"/>
+        <v>33.867803180146439</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="1"/>
+        <v>17031.161881959924</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55">
+        <f t="shared" ref="H55" si="2">_xlfn.STDEV.S(H2:H51)</f>
+        <v>0.8842989683006075</v>
+      </c>
+      <c r="I55">
+        <f t="shared" ref="I55:P55" si="3">_xlfn.STDEV.S(I2:I51)</f>
+        <v>0.35123762572419998</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="3"/>
+        <v>18.211277062438484</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="3"/>
+        <v>9.5199897101642268</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="3"/>
+        <v>1.6033611167959556</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="3"/>
+        <v>0.35971572831067988</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="3"/>
+        <v>427.27782523810606</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="3"/>
+        <v>7.3073961010166348</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="3"/>
+        <v>3238.3627682196397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>